<commit_message>
Add pedidos No perecedero
</commit_message>
<xml_diff>
--- a/Backend/Documents/PedidosNP/Salida/output.xlsx
+++ b/Backend/Documents/PedidosNP/Salida/output.xlsx
@@ -361,7 +361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,17 +397,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aceituna cocktail- Gumendi- 200 gr</t>
+          <t>Alervita- mezcla de hierbas para ALERGIAS- Pamies Vitae - 120 gr</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.16</v>
+        <v>0.08</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -416,7 +416,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aceituna Manzanilla Especias -Gumendi- bote 350 gr</t>
+          <t>Amhepvita - mezcla de hierbas para LIMP. HEPATICA - Pamies vitae - 255 gr</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -435,17 +435,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aceituna Picolimon - Gumendi- bote 350 gr</t>
+          <t>Amrenavita - mezcla de hierbas para LIMP. RENAL - Pamies vitae - 255 gr</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -454,17 +454,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aceituna verdial guindilla - gumendi -  bote gr</t>
+          <t>Biodent Vital- dentifrico- Pamies Vitae- 75 ml</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D5" t="n">
-        <v>0.58</v>
+        <v>3.67</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -473,17 +473,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Aceitunas rellenas de anchoa- Gumendi- 350 gr</t>
+          <t>Champu de Lavanda y Salvia- Pamies Vitae- (200 ml)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D6" t="n">
-        <v>1.42</v>
+        <v>2.17</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -492,17 +492,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Alubia roja - Gumendi - 660 gr</t>
+          <t>Colvita- Mezcla de hierbas para COLESTEROL- Pamies Vitae- 120 gr</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1.33</v>
+        <v>0.33</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -511,17 +511,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Champinon laminado -Gumendi- bote 218 gr</t>
+          <t>Comprimidos de hoja de Estevia + Perilla - 100 unds</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20.39</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -530,14 +530,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Compota de Manzana -Gumendi - bote 720 gr</t>
+          <t>Digevita - mezcla de hierbas para DIGESTION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9099999999999999</v>
+        <v>0.9199999999999999</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -549,17 +549,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Conserva de Acelga al natural - Ekolo-  660 gr</t>
+          <t>Epilobio planta seca - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.51</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -568,17 +568,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conserva de alubias blancas con verduras-Gumendi-720 gr</t>
+          <t>Estevia Fluid -liquido 50 ml- Pamies Vitae</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D11" t="n">
-        <v>2.33</v>
+        <v>1.92</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -587,17 +587,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Conserva de Borraja- Gumendi- bote 660gr</t>
+          <t>Estevia Instant en polvo- Pamies Vitae- 100 gr</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D12" t="n">
-        <v>0.92</v>
+        <v>1.5</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -606,17 +606,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Conserva de cardo al natural - Gumendi- bote 660 gr</t>
+          <t>Esteviatabs - 300 comprimidos de 60 mg- Pamies Vitae</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D13" t="n">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -625,17 +625,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Conserva de garbanzos con verduras-Gumendi-450g</t>
+          <t>Graviola capsulas – Pamies vitae – 100 capsulas</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>19.6</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1.63</v>
+        <v>0.08</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -644,17 +644,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Conserva de Guisantes- Gumendi- 245 gr</t>
+          <t>Graviola en polvo – Pamies vitae – 150 gr</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>2.41</v>
+        <v>0.08</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -663,17 +663,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Conserva de Judia Verde redonda Gumendi 660 gr</t>
+          <t>Hepvita - mezcla de hierbas para HIGADO - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5.94</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.49</v>
+        <v>0.08</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -682,17 +682,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Conserva de Judias al natural  - Gumendi- 660 gr</t>
+          <t>Insovita – mezcla de hierbas IMSONIO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>0.67</v>
+        <v>0.17</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -701,17 +701,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Conserva de lentejas con verduras-Gumendi-625g</t>
+          <t>Levadura arroz rojo- -Pamies Vitae - 60 capsulas</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D18" t="n">
-        <v>1.42</v>
+        <v>1.58</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -720,14 +720,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Conserva Tomate Frito a la Navarra- Gumendi- 340 gr</t>
+          <t>Obvita - mezcla de hierpas para OBESIDAD - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>2.59</v>
+        <v>0.16</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -739,17 +739,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Conserva zanahoria rallada - Gumendi- 345 gr</t>
+          <t>Orivita – mezcla de hierbas INFECCION ORINA – Pamies vitae- 120gr</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5</v>
+        <v>0.16</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -758,17 +758,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fritada (pisto navarro)- Gumendi- 410 gr.</t>
+          <t>Perilla (Perilla frustescens)-Pamies Vitae-100gr</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.34</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -777,17 +777,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Macedonia de Verduras -Gumendi -660 gramos</t>
+          <t>Resvita – mezcla de hierbas CONSTIPADO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.58</v>
+        <v>0.08</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -796,14 +796,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mermelada kiwi- Gumendi- bote 280 gr</t>
+          <t>Revita - mezcla de hierbas para RIÑON - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>0.42</v>
+        <v>0.25</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -815,17 +815,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pimiento morron extra tiras - Gumendi- bote 215 gr</t>
+          <t>Spray Nasal 100% agua de mar-Pamies Vitae-50ml</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0.59</v>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -834,17 +834,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pimiento piquillo entero extra- Gumendi- 215 gr</t>
+          <t>Stevia comprimidos - Pamies Vitae-100 unds</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>1.08</v>
+        <v>0.75</v>
       </c>
       <c r="E25" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -853,17 +853,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Pimiento piquillo rojo tiras - Gumendi- bote 185 gr</t>
+          <t>Stevia, planta seca - Pamies Vitae- sobre 120 gramos</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5</v>
+        <v>0.84</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -872,17 +872,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Polvorones blancos-Pasteco- 300 gr</t>
+          <t>Tomillo-Planta seca-Pamies vitae-120 gr</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>1.16</v>
+        <v>0.08</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -891,17 +891,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Polvorones de Chocolate -Pasteco- 300 gr (12 unidades)</t>
+          <t>Allergyvita - Pamies Vitae - 120gr</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>1.25</v>
+        <v>0.08</v>
       </c>
       <c r="E28" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -910,17 +910,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sal de salinas de oro-Gumendi-400g</t>
+          <t>BERRUGUERA - Celidonium Majus - Pamies Vitae - bolsa 120 gr</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0.17</v>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -929,17 +929,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Salsa de tomate frito- Gumendi- 315 gr</t>
+          <t>Cabellovita "Hierbas fortalecimiento del CABELLO y contra la caida"- PAMIES VITAE- 120 gr</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>3.17</v>
+        <v>0.17</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -948,17 +948,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tomate entero pelado- Gumendi- 660g</t>
+          <t>Diente de leon planta seca - Pamies vitae - 100gr</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>3.17</v>
+        <v>0.08</v>
       </c>
       <c r="E31" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -967,14 +967,14 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tomate triturado- Gumendi-660gr</t>
+          <t>Hipervita - mezcla de hierbas para HIPERTENSION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>33.83</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>2.82</v>
+        <v>0.08</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -986,74 +986,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Brotes de ajo- Gumendi- 240 gr</t>
+          <t>Stevia rebaudiana - Pamies Vitae - bolsa 500 gr</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Cava Brut Natura- Marrugat - Pinerd - Penedes</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>DESCATALOGADO - Turron Alicante (duro)- Delicatalia- Abuelo- 150 gr</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Escalivada - Gumendi - 320gr</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>7</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,17 +1046,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aceituna cocktail- Gumendi- 200 gr</t>
+          <t>Biodent Vital- dentifrico- Pamies Vitae- 75 ml</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>1.33</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -1122,17 +1065,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aceituna Manzanilla Especias -Gumendi- bote 350 gr</t>
+          <t>Champu de Lavanda y Salvia- Pamies Vitae- (200 ml)</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -1141,17 +1084,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aceituna Picolimon - Gumendi- bote 350 gr</t>
+          <t>Digevita - mezcla de hierbas para DIGESTION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>1.33</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1160,17 +1103,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aceituna verdial guindilla - gumendi -  bote gr</t>
+          <t>Estevia Fluid -liquido 50 ml- Pamies Vitae</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -1179,17 +1122,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Alubia roja - Gumendi - 660 gr</t>
+          <t>Estevia Instant en polvo- Pamies Vitae- 100 gr</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>1.66</v>
+        <v>4.67</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -1198,17 +1141,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bote de seta shiitake- Gumendi- 240 gr</t>
+          <t>Esteviatabs - 300 comprimidos de 60 mg- Pamies Vitae</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.13</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04</v>
+        <v>1.66</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1217,17 +1160,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Brotes de ajo- Gumendi- 240 gr</t>
+          <t>Orivita – mezcla de hierbas INFECCION ORINA – Pamies vitae- 120gr</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1236,17 +1179,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Champinon laminado -Gumendi- bote 218 gr</t>
+          <t>Stevia comprimidos - Pamies Vitae-100 unds</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2.67</v>
+        <v>0.67</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -1255,17 +1198,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Compota de Manzana -Gumendi - bote 720 gr</t>
+          <t>Stevia, planta seca - Pamies Vitae- sobre 120 gramos</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>2.67</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1274,17 +1217,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conserva de Acelga al natural - Ekolo-  660 gr</t>
+          <t>Tomillo-Planta seca-Pamies vitae-120 gr</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>1.33</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1293,17 +1236,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Conserva de alubias blancas con verduras-Gumendi-720 gr</t>
+          <t>Cabellovita "Hierbas fortalecimiento del CABELLO y contra la caida"- PAMIES VITAE- 120 gr</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1312,17 +1255,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Conserva de Borraja- Gumendi- bote 660gr</t>
+          <t>Colvita- Mezcla de hierbas para COLESTEROL- Pamies Vitae- 120 gr</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>1.34</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1331,17 +1274,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Conserva de cardo al natural - Gumendi- bote 660 gr</t>
+          <t>Epilobio planta seca - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1350,17 +1293,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Conserva de garbanzos con verduras-Gumendi-450g</t>
+          <t>Levadura arroz rojo- -Pamies Vitae - 60 capsulas</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>2.67</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1369,435 +1312,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Conserva de Guisantes- Gumendi- 245 gr</t>
+          <t>Resvita – mezcla de hierbas CONSTIPADO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>5.67</v>
+        <v>0.67</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Conserva de Judias al natural  - Gumendi- 660 gr</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>13</v>
-      </c>
-      <c r="D17" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="E17" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Conserva de lentejas con verduras-Gumendi-625g</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Conserva Tomate Frito a la Navarra- Gumendi- 340 gr</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>13</v>
-      </c>
-      <c r="D19" t="n">
-        <v>4.34</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Escalivada - Gumendi - 320gr</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Macedonia de Verduras -Gumendi -660 gramos</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>6</v>
-      </c>
-      <c r="D21" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Mermelada kiwi- Gumendi- bote 280 gr</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Pimiento morron extra tiras - Gumendi- bote 215 gr</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>10</v>
-      </c>
-      <c r="D23" t="n">
-        <v>3.33</v>
-      </c>
-      <c r="E23" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Pimiento piquillo entero extra- Gumendi- 215 gr</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E24" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Polvorones blancos-Pasteco- 300 gr</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E25" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Polvorones de Chocolate -Pasteco- 300 gr (12 unidades)</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Sal de salinas de oro-Gumendi-400g</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>7</v>
-      </c>
-      <c r="D27" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="E27" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Salsa de tomate frito- Gumendi- 315 gr</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>23</v>
-      </c>
-      <c r="D28" t="n">
-        <v>7.66</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Tomate entero pelado- Gumendi- 660g</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>38</v>
-      </c>
-      <c r="D29" t="n">
-        <v>12.67</v>
-      </c>
-      <c r="E29" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Tomate triturado- Gumendi-660gr</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>8</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2.66</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Aceitunas rellenas de anchoa- Gumendi- 350 gr</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Cava Brut Natura- Marrugat - Pinerd - Penedes</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Conserva zanahoria rallada - Gumendi- 345 gr</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>3</v>
-      </c>
-      <c r="D33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>DESCATALOGADO - Turron Alicante (duro)- Delicatalia- Abuelo- 150 gr</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>2</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Fritada (pisto navarro)- Gumendi- 410 gr.</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Menestra de Verdura -Gumendi- bote 380 gr.</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E36" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Pimiento piquillo rojo tiras - Gumendi- bote 185 gr</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E37" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Remolacha roja rallada- Gumendi- bote 345 gr</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>2</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E38" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1811,7 +1336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1847,17 +1372,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aceituna cocktail- Gumendi- 200 gr</t>
+          <t>Allergyvita - Pamies Vitae - 120gr</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.33</v>
+        <v>0.33</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1866,14 +1391,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aceituna verdial guindilla - gumendi -  bote gr</t>
+          <t>Amrenavita - mezcla de hierbas para LIMP. RENAL - Pamies vitae - 255 gr</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.33</v>
+        <v>0.66</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1885,17 +1410,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aceitunas rellenas de anchoa- Gumendi- 350 gr</t>
+          <t>Biodent Vital- dentifrico- Pamies Vitae- 75 ml</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>2.67</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -1904,17 +1429,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Brotes de ajo- Gumendi- 240 gr</t>
+          <t>Champu de Lavanda y Salvia- Pamies Vitae- (200 ml)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>0.33</v>
+        <v>1.66</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -1923,7 +1448,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cava Brut Natura- Marrugat - Pinerd - Penedes</t>
+          <t>Diente de leon planta seca - Pamies vitae - 100gr</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1942,14 +1467,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Compota de Manzana -Gumendi - bote 720 gr</t>
+          <t>Digevita - mezcla de hierbas para DIGESTION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>2.66</v>
+        <v>1.66</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1961,17 +1486,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Conserva de alubias blancas con verduras-Gumendi-720 gr</t>
+          <t>Estevia Fluid -liquido 50 ml- Pamies Vitae</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -1980,17 +1505,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Conserva de Borraja- Gumendi- bote 660gr</t>
+          <t>Estevia Instant en polvo- Pamies Vitae- 100 gr</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -1999,17 +1524,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Conserva de cardo al natural - Gumendi- bote 660 gr</t>
+          <t>Esteviatabs - 300 comprimidos de 60 mg- Pamies Vitae</t>
         </is>
       </c>
       <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
         <v>3</v>
       </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -2018,17 +1543,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conserva de garbanzos con verduras-Gumendi-450g</t>
+          <t>Stevia, planta seca - Pamies Vitae- sobre 120 gramos</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>11.6</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>3.86</v>
+        <v>0.66</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -2037,17 +1562,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Conserva de Guisantes- Gumendi- 245 gr</t>
+          <t>Colvita- Mezcla de hierbas para COLESTEROL- Pamies Vitae- 120 gr</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>0.33</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2056,17 +1581,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Conserva de Judias al natural  - Gumendi- 660 gr</t>
+          <t>Graviola capsulas – Pamies vitae – 100 capsulas</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2075,14 +1600,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Conserva de lentejas con verduras-Gumendi-625g</t>
+          <t>Insovita – mezcla de hierbas IMSONIO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.67</v>
+        <v>0.33</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -2094,17 +1619,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Conserva Tomate Frito a la Navarra- Gumendi- 340 gr</t>
+          <t>Levadura arroz rojo- -Pamies Vitae - 60 capsulas</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>3.33</v>
+        <v>1.33</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -2113,7 +1638,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DESCATALOGADO - Turron Alicante (duro)- Delicatalia- Abuelo- 150 gr</t>
+          <t>Revita - mezcla de hierbas para RIÑON - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -2132,17 +1657,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Escalivada - Gumendi - 320gr</t>
+          <t>Stevia comprimidos - Pamies Vitae-100 unds</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>0.33</v>
+        <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -2151,7 +1676,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Fritada (pisto navarro)- Gumendi- 410 gr.</t>
+          <t>Tomillo-Planta seca-Pamies vitae-120 gr</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -2162,291 +1687,6 @@
       </c>
       <c r="E18" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Macedonia de Verduras -Gumendi -660 gramos</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>4</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Pimiento morron extra tiras - Gumendi- bote 215 gr</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2.67</v>
-      </c>
-      <c r="E20" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Pimiento piquillo rojo tiras - Gumendi- bote 185 gr</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>5</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.66</v>
-      </c>
-      <c r="E21" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Polvorones blancos-Pasteco- 300 gr</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>9</v>
-      </c>
-      <c r="D22" t="n">
-        <v>3</v>
-      </c>
-      <c r="E22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Polvorones de Chocolate -Pasteco- 300 gr (12 unidades)</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>9</v>
-      </c>
-      <c r="D23" t="n">
-        <v>3</v>
-      </c>
-      <c r="E23" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Sal de salinas de oro-Gumendi-400g</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>5</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="E24" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Salsa de tomate frito- Gumendi- 315 gr</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>16</v>
-      </c>
-      <c r="D25" t="n">
-        <v>5.33</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Tomate entero pelado- Gumendi- 660g</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>24</v>
-      </c>
-      <c r="D26" t="n">
-        <v>8</v>
-      </c>
-      <c r="E26" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Tomate triturado- Gumendi-660gr</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>17.83</v>
-      </c>
-      <c r="D27" t="n">
-        <v>5.95</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Aceituna Manzanilla Especias -Gumendi- bote 350 gr</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Alubia roja - Gumendi - 660 gr</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>2</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Champinon laminado -Gumendi- bote 218 gr</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="E30" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Conserva de Acelga al natural - Ekolo-  660 gr</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="E31" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Conserva de Judia Verde redonda Gumendi 660 gr</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E32" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Conserva zanahoria rallada - Gumendi- 345 gr</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E33" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2460,7 +1700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2501,20 +1741,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aceituna cocktail- Gumendi- 200 gr</t>
+          <t>Alervita- mezcla de hierbas para ALERGIAS- Pamies Vitae - 120 gr</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.16</v>
+        <v>0.08</v>
       </c>
       <c r="D2" t="n">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2523,17 +1763,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aceituna Manzanilla Especias -Gumendi- bote 350 gr</t>
+          <t>Amhepvita - mezcla de hierbas para LIMP. HEPATICA - Pamies vitae - 255 gr</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>0.08</v>
       </c>
       <c r="D3" t="n">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -2545,20 +1785,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aceituna Picolimon - Gumendi- bote 350 gr</t>
+          <t>Amrenavita - mezcla de hierbas para LIMP. RENAL - Pamies vitae - 255 gr</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2567,20 +1807,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aceituna verdial guindilla - gumendi -  bote gr</t>
+          <t>Biodent Vital- dentifrico- Pamies Vitae- 75 ml</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.58</v>
+        <v>3.67</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>0.33</v>
+        <v>2.67</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -2589,20 +1829,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Aceitunas rellenas de anchoa- Gumendi- 350 gr</t>
+          <t>Champu de Lavanda y Salvia- Pamies Vitae- (200 ml)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.42</v>
+        <v>2.17</v>
       </c>
       <c r="D6" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>1.66</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -2611,20 +1851,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Alubia roja - Gumendi - 660 gr</t>
+          <t>Colvita- Mezcla de hierbas para COLESTEROL- Pamies Vitae- 120 gr</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.33</v>
+        <v>0.33</v>
       </c>
       <c r="D7" t="n">
-        <v>1.66</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.67</v>
+        <v>0.33</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2633,20 +1873,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Champinon laminado -Gumendi- bote 218 gr</t>
+          <t>Comprimidos de hoja de Estevia + Perilla - 100 unds</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.7</v>
+        <v>0.5</v>
       </c>
       <c r="D8" t="n">
-        <v>2.67</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>2.83</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2655,17 +1895,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Compota de Manzana -Gumendi - bote 720 gr</t>
+          <t>Digevita - mezcla de hierbas para DIGESTION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9099999999999999</v>
+        <v>0.9199999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>2.67</v>
+        <v>1.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.66</v>
+        <v>1.66</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2677,20 +1917,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Conserva de Acelga al natural - Ekolo-  660 gr</t>
+          <t>Epilobio planta seca - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E10" t="n">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2699,20 +1939,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Conserva de alubias blancas con verduras-Gumendi-720 gr</t>
+          <t>Estevia Fluid -liquido 50 ml- Pamies Vitae</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2.33</v>
+        <v>1.92</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -2721,20 +1961,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Conserva de Borraja- Gumendi- bote 660gr</t>
+          <t>Estevia Instant en polvo- Pamies Vitae- 100 gr</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.92</v>
+        <v>1.5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.34</v>
+        <v>4.67</v>
       </c>
       <c r="E12" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -2743,20 +1983,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Conserva de cardo al natural - Gumendi- bote 660 gr</t>
+          <t>Esteviatabs - 300 comprimidos de 60 mg- Pamies Vitae</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="D13" t="n">
-        <v>0.66</v>
+        <v>1.66</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -2765,20 +2005,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Conserva de garbanzos con verduras-Gumendi-450g</t>
+          <t>Graviola capsulas – Pamies vitae – 100 capsulas</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.63</v>
+        <v>0.08</v>
       </c>
       <c r="D14" t="n">
-        <v>2.67</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>3.86</v>
+        <v>0.33</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2787,20 +2027,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Conserva de Guisantes- Gumendi- 245 gr</t>
+          <t>Graviola en polvo – Pamies vitae – 150 gr</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.41</v>
+        <v>0.08</v>
       </c>
       <c r="D15" t="n">
-        <v>5.67</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2809,20 +2049,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Conserva de Judia Verde redonda Gumendi 660 gr</t>
+          <t>Hepvita - mezcla de hierbas para HIGADO - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.49</v>
+        <v>0.08</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2831,20 +2071,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Conserva de Judias al natural  - Gumendi- 660 gr</t>
+          <t>Insovita – mezcla de hierbas IMSONIO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.67</v>
+        <v>0.17</v>
       </c>
       <c r="D17" t="n">
-        <v>4.33</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>0.33</v>
       </c>
       <c r="F17" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2853,20 +2093,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Conserva de lentejas con verduras-Gumendi-625g</t>
+          <t>Levadura arroz rojo- -Pamies Vitae - 60 capsulas</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.42</v>
+        <v>1.58</v>
       </c>
       <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="n">
         <v>1.33</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.67</v>
-      </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -2875,17 +2115,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Conserva Tomate Frito a la Navarra- Gumendi- 340 gr</t>
+          <t>Obvita - mezcla de hierpas para OBESIDAD - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.59</v>
+        <v>0.16</v>
       </c>
       <c r="D19" t="n">
-        <v>4.34</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>3.33</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2897,20 +2137,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Conserva zanahoria rallada - Gumendi- 345 gr</t>
+          <t>Orivita – mezcla de hierbas INFECCION ORINA – Pamies vitae- 120gr</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.5</v>
+        <v>0.16</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -2919,20 +2159,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fritada (pisto navarro)- Gumendi- 410 gr.</t>
+          <t>Perilla (Perilla frustescens)-Pamies Vitae-100gr</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0.34</v>
       </c>
       <c r="D21" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -2941,20 +2181,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Macedonia de Verduras -Gumendi -660 gramos</t>
+          <t>Resvita – mezcla de hierbas CONSTIPADO – Pamies vitae – 120 gr</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.58</v>
+        <v>0.08</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>0.67</v>
       </c>
       <c r="E22" t="n">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2963,17 +2203,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mermelada kiwi- Gumendi- bote 280 gr</t>
+          <t>Revita - mezcla de hierbas para RIÑON - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.42</v>
+        <v>0.25</v>
       </c>
       <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.33</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -2985,20 +2225,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pimiento morron extra tiras - Gumendi- bote 215 gr</t>
+          <t>Spray Nasal 100% agua de mar-Pamies Vitae-50ml</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0.59</v>
       </c>
       <c r="D24" t="n">
-        <v>3.33</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>2.67</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3007,20 +2247,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pimiento piquillo entero extra- Gumendi- 215 gr</t>
+          <t>Stevia comprimidos - Pamies Vitae-100 unds</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.08</v>
+        <v>0.75</v>
       </c>
       <c r="D25" t="n">
-        <v>1.33</v>
+        <v>0.67</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -3029,20 +2269,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Pimiento piquillo rojo tiras - Gumendi- bote 185 gr</t>
+          <t>Stevia, planta seca - Pamies Vitae- sobre 120 gramos</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5</v>
+        <v>0.84</v>
       </c>
       <c r="D26" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>1.66</v>
+        <v>0.66</v>
       </c>
       <c r="F26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -3051,20 +2291,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Polvorones blancos-Pasteco- 300 gr</t>
+          <t>Tomillo-Planta seca-Pamies vitae-120 gr</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.16</v>
+        <v>0.08</v>
       </c>
       <c r="D27" t="n">
         <v>1.33</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -3073,20 +2313,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Polvorones de Chocolate -Pasteco- 300 gr (12 unidades)</t>
+          <t>Allergyvita - Pamies Vitae - 120gr</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.25</v>
+        <v>0.08</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="F28" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -3095,20 +2335,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sal de salinas de oro-Gumendi-400g</t>
+          <t>BERRUGUERA - Celidonium Majus - Pamies Vitae - bolsa 120 gr</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0.17</v>
       </c>
       <c r="D29" t="n">
-        <v>2.33</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>1.67</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -3117,20 +2357,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Salsa de tomate frito- Gumendi- 315 gr</t>
+          <t>Cabellovita "Hierbas fortalecimiento del CABELLO y contra la caida"- PAMIES VITAE- 120 gr</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.17</v>
+        <v>0.17</v>
       </c>
       <c r="D30" t="n">
-        <v>7.66</v>
+        <v>0.33</v>
       </c>
       <c r="E30" t="n">
-        <v>5.33</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -3139,20 +2379,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tomate entero pelado- Gumendi- 660g</t>
+          <t>Diente de leon planta seca - Pamies vitae - 100gr</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.17</v>
+        <v>0.08</v>
       </c>
       <c r="D31" t="n">
-        <v>12.67</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>0.33</v>
       </c>
       <c r="F31" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3161,17 +2401,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tomate triturado- Gumendi-660gr</t>
+          <t>Hipervita - mezcla de hierbas para HIPERTENSION - Pamies vitae - 120 gr</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.82</v>
+        <v>0.08</v>
       </c>
       <c r="D32" t="n">
-        <v>2.66</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>5.95</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -3183,152 +2423,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Brotes de ajo- Gumendi- 240 gr</t>
+          <t>Stevia rebaudiana - Pamies Vitae - bolsa 500 gr</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="D33" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Cava Brut Natura- Marrugat - Pinerd - Penedes</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>DESCATALOGADO - Turron Alicante (duro)- Delicatalia- Abuelo- 150 gr</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Escalivada - Gumendi - 320gr</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="D36" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F36" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Bote de seta shiitake- Gumendi- 240 gr</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Menestra de Verdura -Gumendi- bote 380 gr.</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Remolacha roja rallada- Gumendi- bote 345 gr</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved bugs with providers
</commit_message>
<xml_diff>
--- a/Backend/Documents/PedidosNP/Salida/output.xlsx
+++ b/Backend/Documents/PedidosNP/Salida/output.xlsx
@@ -361,7 +361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,10 +370,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre_producto</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
@@ -397,36 +395,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brick leche UHT Entera - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2429</v>
-      </c>
-      <c r="D2" t="n">
-        <v>202.41</v>
-      </c>
-      <c r="E2" t="n">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Brick leche UHT Semidesnatada - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1386</v>
-      </c>
-      <c r="D3" t="n">
-        <v>115.5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>406</v>
+          <t>No hay ventas en este periodo</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -440,7 +410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,10 +419,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre_producto</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
@@ -476,36 +444,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brick leche UHT Entera - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>729</v>
-      </c>
-      <c r="D2" t="n">
-        <v>243</v>
-      </c>
-      <c r="E2" t="n">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Brick leche UHT Semidesnatada - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>298</v>
-      </c>
-      <c r="D3" t="n">
-        <v>99.33</v>
-      </c>
-      <c r="E3" t="n">
-        <v>406</v>
+          <t>No hay ventas en este periodo</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -519,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,10 +468,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre_producto</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
@@ -555,36 +493,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brick leche UHT Entera - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>728</v>
-      </c>
-      <c r="D2" t="n">
-        <v>242.67</v>
-      </c>
-      <c r="E2" t="n">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Brick leche UHT Semidesnatada - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>236</v>
-      </c>
-      <c r="D3" t="n">
-        <v>78.66</v>
-      </c>
-      <c r="E3" t="n">
-        <v>406</v>
+          <t>No hay ventas en este periodo</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -598,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,24 +517,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>3mo_pre_mensual</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>3mo_post_mensual</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>descripcion</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>12mo_mensual</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>3mo_pre_mensual</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>3mo_post_mensual</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -639,42 +547,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brick leche UHT Entera - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>202.41</v>
-      </c>
-      <c r="D2" t="n">
-        <v>243</v>
-      </c>
-      <c r="E2" t="n">
-        <v>242.67</v>
-      </c>
-      <c r="F2" t="n">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Brick leche UHT Semidesnatada - El Buen Pastor - 1L</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>115.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>99.33</v>
-      </c>
-      <c r="E3" t="n">
-        <v>78.66</v>
-      </c>
-      <c r="F3" t="n">
-        <v>406</v>
+          <t>No hay ventas en este periodo</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>